<commit_message>
EC1: Updates on Markov models to add more preventive maintenance scenarios.
</commit_message>
<xml_diff>
--- a/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Quantitative Models/Compiled Safety Results.xlsx
+++ b/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Quantitative Models/Compiled Safety Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>ResNet</t>
   </si>
@@ -60,9 +60,6 @@
     <t>RS1.3</t>
   </si>
   <si>
-    <t>15 years without 2-year preventive maintenance</t>
-  </si>
-  <si>
     <t>Operational Context</t>
   </si>
   <si>
@@ -73,6 +70,39 @@
   </si>
   <si>
     <t>With 2-Year Preventive Maintenance</t>
+  </si>
+  <si>
+    <t>15 years without preventive maintenance</t>
+  </si>
+  <si>
+    <t>15 years with 1-year preventive maintenance</t>
+  </si>
+  <si>
+    <t>15 years with 2-year preventive maintenance (all failed states)</t>
+  </si>
+  <si>
+    <t>15 years with 1-year preventive maintenance (all failed states)</t>
+  </si>
+  <si>
+    <t>With 2-Year Preventive Maintenance (All Failed States)</t>
+  </si>
+  <si>
+    <t>With 1-Year Preventive Maintenance</t>
+  </si>
+  <si>
+    <t>With 1-Year Preventive Maintenance (All Failed States)</t>
+  </si>
+  <si>
+    <t>With 6-Month Preventive Maintenance</t>
+  </si>
+  <si>
+    <t>15 years with 6-month preventive maintenance</t>
+  </si>
+  <si>
+    <t>15 years with 6-month preventive maintenance (all failed states)</t>
+  </si>
+  <si>
+    <t>With 6-Month Preventive Maintenance (All Failed States)</t>
   </si>
 </sst>
 </file>
@@ -538,6 +568,27 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -558,23 +609,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -879,7 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -891,21 +925,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="23" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="25"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
+      <c r="A2" s="29"/>
       <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
@@ -1039,21 +1073,21 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="23" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="32"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="14" t="s">
         <v>4</v>
       </c>
@@ -1187,21 +1221,21 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="23" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="25"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="14" t="s">
         <v>4</v>
       </c>
@@ -1335,10 +1369,10 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="27"/>
+      <c r="B25" s="34"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
@@ -1400,21 +1434,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>15</v>
+      <c r="A1" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>4</v>
@@ -1425,24 +1459,79 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1">
-        <v>0.98794463362677976</v>
+        <v>0.98794046805355373</v>
       </c>
       <c r="C2" s="1">
-        <v>1.2055366368170395E-2</v>
+        <v>1.2059531941354725E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
-        <v>0.99829871494893663</v>
+        <v>0.99829856113814031</v>
       </c>
       <c r="C3" s="1">
-        <v>1.7012850459721797E-3</v>
+        <v>1.7014388567486464E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.99829951526389349</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.7004847310063409E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.99909783484082615</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9.0216515254284545E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.99909972824658</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9.0027174691362059E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.99949834440802843</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5.0165559341496999E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.99950206411061682</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4.9793588229815665E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1453,93 +1542,213 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:8" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="D1" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="22">
         <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.93138253107898927</v>
+        <v>0.93137860399441119</v>
       </c>
       <c r="C2" s="12">
         <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.94114381743106557</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.94114367242629116</v>
+      </c>
+      <c r="D2" s="12">
+        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$4</f>
+        <v>0.94114457192615042</v>
+      </c>
+      <c r="E2" s="12">
+        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$5</f>
+        <v>0.94189718587116866</v>
+      </c>
+      <c r="F2" s="12">
+        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$6</f>
+        <v>0.94189897087508834</v>
+      </c>
+      <c r="G2" s="12">
+        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$7</f>
+        <v>0.94227476534447663</v>
+      </c>
+      <c r="H2" s="12">
+        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$8</f>
+        <v>0.94227827208553649</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="23">
         <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.98769290533413168</v>
+        <v>0.98768874082229374</v>
       </c>
       <c r="C3" s="1">
         <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.99804434843636769</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.99804419466476235</v>
+      </c>
+      <c r="D3" s="12">
+        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$4</f>
+        <v>0.99804514854740423</v>
+      </c>
+      <c r="E3" s="12">
+        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$5</f>
+        <v>0.99884326471250873</v>
+      </c>
+      <c r="F3" s="12">
+        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$6</f>
+        <v>0.99884515763582282</v>
+      </c>
+      <c r="G3" s="12">
+        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$7</f>
+        <v>0.99924367222987331</v>
+      </c>
+      <c r="H3" s="12">
+        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$8</f>
+        <v>0.99924739098468141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="23">
         <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.98594681198865974</v>
+        <v>0.98594265483905585</v>
       </c>
       <c r="C4" s="1">
         <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.99627995528756697</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.99627980178780673</v>
+      </c>
+      <c r="D4" s="12">
+        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$4</f>
+        <v>0.99628075398412685</v>
+      </c>
+      <c r="E4" s="12">
+        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$5</f>
+        <v>0.99707745919921109</v>
+      </c>
+      <c r="F4" s="12">
+        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$6</f>
+        <v>0.99707934877611981</v>
+      </c>
+      <c r="G4" s="12">
+        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$7</f>
+        <v>0.99747715885596655</v>
+      </c>
+      <c r="H4" s="12">
+        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$8</f>
+        <v>0.99748087103657235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="23">
         <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.9371136966931215</v>
+        <v>0.93710974544363668</v>
       </c>
       <c r="C5" s="1">
         <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.94693504810635587</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.94693490220930954</v>
+      </c>
+      <c r="D5" s="12">
+        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$4</f>
+        <v>0.94693580724414783</v>
+      </c>
+      <c r="E5" s="12">
+        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$5</f>
+        <v>0.94769305232086376</v>
+      </c>
+      <c r="F5" s="12">
+        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$6</f>
+        <v>0.9476948483086195</v>
+      </c>
+      <c r="G5" s="12">
+        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$7</f>
+        <v>0.94807295519022206</v>
+      </c>
+      <c r="H5" s="12">
+        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$8</f>
+        <v>0.94807648350964857</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="23">
         <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.98037816326675897</v>
+        <v>0.98037402959682518</v>
       </c>
       <c r="C6" s="1">
         <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.99065294475088572</v>
+        <v>0.99065279211809554</v>
+      </c>
+      <c r="D6" s="12">
+        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$4</f>
+        <v>0.99065373893639042</v>
+      </c>
+      <c r="E6" s="12">
+        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$5</f>
+        <v>0.99144594434334732</v>
+      </c>
+      <c r="F6" s="12">
+        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$6</f>
+        <v>0.99144782324788516</v>
+      </c>
+      <c r="G6" s="12">
+        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$7</f>
+        <v>0.99184338648787629</v>
+      </c>
+      <c r="H6" s="12">
+        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$8</f>
+        <v>0.99184707770200642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EC1:Quantitative models adapted to high demand. Safety models were updated to take into account that the system operates high IEC61508:2010 high demand instead of low demand.
</commit_message>
<xml_diff>
--- a/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Quantitative Models/Compiled Safety Results.xlsx
+++ b/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Quantitative Models/Compiled Safety Results.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio\Documents\safetyartist GitHub\EC1-ECG_Analysis\ecg_oversampling\safetyArtist\Quantitative Models\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="20730" windowHeight="10050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Safety Prob. Systematic Faults" sheetId="8" r:id="rId1"/>
-    <sheet name="Safety Prob. Random Faults" sheetId="9" r:id="rId2"/>
-    <sheet name="Safety Prob. Final" sheetId="10" r:id="rId3"/>
+    <sheet name="Unsafe F. Rate Random Faults" sheetId="9" r:id="rId2"/>
+    <sheet name="Final Unsafe Failure Rates" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>ResNet</t>
   </si>
@@ -63,46 +68,16 @@
     <t>Operational Context</t>
   </si>
   <si>
-    <t>15 years with 2-year preventive maintenance</t>
-  </si>
-  <si>
     <t>Without Preventive Maintenance</t>
   </si>
   <si>
-    <t>With 2-Year Preventive Maintenance</t>
-  </si>
-  <si>
-    <t>15 years without preventive maintenance</t>
-  </si>
-  <si>
-    <t>15 years with 1-year preventive maintenance</t>
-  </si>
-  <si>
-    <t>15 years with 2-year preventive maintenance (all failed states)</t>
-  </si>
-  <si>
-    <t>15 years with 1-year preventive maintenance (all failed states)</t>
-  </si>
-  <si>
-    <t>With 2-Year Preventive Maintenance (All Failed States)</t>
-  </si>
-  <si>
-    <t>With 1-Year Preventive Maintenance</t>
-  </si>
-  <si>
-    <t>With 1-Year Preventive Maintenance (All Failed States)</t>
-  </si>
-  <si>
-    <t>With 6-Month Preventive Maintenance</t>
-  </si>
-  <si>
-    <t>15 years with 6-month preventive maintenance</t>
-  </si>
-  <si>
-    <t>15 years with 6-month preventive maintenance (all failed states)</t>
-  </si>
-  <si>
-    <t>With 6-Month Preventive Maintenance (All Failed States)</t>
+    <t>MTTUF (lower bound)</t>
+  </si>
+  <si>
+    <t>Unsafe Failure Rate (upper bound)</t>
+  </si>
+  <si>
+    <t>Without preventive maintenance</t>
   </si>
 </sst>
 </file>
@@ -182,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -339,174 +314,118 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -526,42 +445,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -571,44 +490,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,6 +526,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -667,7 +577,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -702,7 +612,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -913,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -925,21 +835,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="30" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="32"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
@@ -1073,21 +983,21 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="30" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="14" t="s">
         <v>4</v>
       </c>
@@ -1221,21 +1131,21 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="30" t="s">
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="32"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="29"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="14" t="s">
         <v>4</v>
       </c>
@@ -1369,10 +1279,10 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="34"/>
+      <c r="B25" s="28"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
@@ -1434,16 +1344,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1451,10 +1362,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1462,76 +1373,11 @@
         <v>18</v>
       </c>
       <c r="B2" s="1">
-        <v>0.98794046805355373</v>
+        <v>57179505.361074015</v>
       </c>
       <c r="C2" s="1">
-        <v>1.2059531941354725E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.99829856113814031</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.7014388567486464E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.99829951526389349</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.7004847310063409E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.99909783484082615</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9.0216515254284545E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.99909972824658</v>
-      </c>
-      <c r="C6" s="1">
-        <v>9.0027174691362059E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.99949834440802843</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5.0165559341496999E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.99950206411061682</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4.9793588229815665E-4</v>
+        <f>1/B2</f>
+        <v>1.7488783676690706E-8</v>
       </c>
     </row>
   </sheetData>
@@ -1542,213 +1388,69 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="37.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
-    <col min="8" max="8" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="B1" s="30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22">
-        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.93137860399441119</v>
-      </c>
-      <c r="C2" s="12">
-        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.94114367242629116</v>
-      </c>
-      <c r="D2" s="12">
-        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$4</f>
-        <v>0.94114457192615042</v>
-      </c>
-      <c r="E2" s="12">
-        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$5</f>
-        <v>0.94189718587116866</v>
-      </c>
-      <c r="F2" s="12">
-        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$6</f>
-        <v>0.94189897087508834</v>
-      </c>
-      <c r="G2" s="12">
-        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$7</f>
-        <v>0.94227476534447663</v>
-      </c>
-      <c r="H2" s="12">
-        <f>'Safety Prob. Systematic Faults'!B26*'Safety Prob. Random Faults'!$B$8</f>
-        <v>0.94227827208553649</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="B2" s="1">
+        <f>'Safety Prob. Systematic Faults'!B26*'Unsafe F. Rate Random Faults'!$C$2</f>
+        <v>1.6487510586997705E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23">
-        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.98768874082229374</v>
-      </c>
-      <c r="C3" s="1">
-        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.99804419466476235</v>
-      </c>
-      <c r="D3" s="12">
-        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$4</f>
-        <v>0.99804514854740423</v>
-      </c>
-      <c r="E3" s="12">
-        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$5</f>
-        <v>0.99884326471250873</v>
-      </c>
-      <c r="F3" s="12">
-        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$6</f>
-        <v>0.99884515763582282</v>
-      </c>
-      <c r="G3" s="12">
-        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$7</f>
-        <v>0.99924367222987331</v>
-      </c>
-      <c r="H3" s="12">
-        <f>'Safety Prob. Systematic Faults'!B27*'Safety Prob. Random Faults'!$B$8</f>
-        <v>0.99924739098468141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="B3" s="1">
+        <f>'Safety Prob. Systematic Faults'!B27*'Unsafe F. Rate Random Faults'!$C$2</f>
+        <v>1.7484327534609885E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="23">
-        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.98594265483905585</v>
-      </c>
-      <c r="C4" s="1">
-        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.99627980178780673</v>
-      </c>
-      <c r="D4" s="12">
-        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$4</f>
-        <v>0.99628075398412685</v>
-      </c>
-      <c r="E4" s="12">
-        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$5</f>
-        <v>0.99707745919921109</v>
-      </c>
-      <c r="F4" s="12">
-        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$6</f>
-        <v>0.99707934877611981</v>
-      </c>
-      <c r="G4" s="12">
-        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$7</f>
-        <v>0.99747715885596655</v>
-      </c>
-      <c r="H4" s="12">
-        <f>'Safety Prob. Systematic Faults'!B28*'Safety Prob. Random Faults'!$B$8</f>
-        <v>0.99748087103657235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="B4" s="1">
+        <f>'Safety Prob. Systematic Faults'!B28*'Unsafe F. Rate Random Faults'!$C$2</f>
+        <v>1.7453417858339704E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="23">
-        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.93710974544363668</v>
-      </c>
-      <c r="C5" s="1">
-        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.94693490220930954</v>
-      </c>
-      <c r="D5" s="12">
-        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$4</f>
-        <v>0.94693580724414783</v>
-      </c>
-      <c r="E5" s="12">
-        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$5</f>
-        <v>0.94769305232086376</v>
-      </c>
-      <c r="F5" s="12">
-        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$6</f>
-        <v>0.9476948483086195</v>
-      </c>
-      <c r="G5" s="12">
-        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$7</f>
-        <v>0.94807295519022206</v>
-      </c>
-      <c r="H5" s="12">
-        <f>'Safety Prob. Systematic Faults'!B29*'Safety Prob. Random Faults'!$B$8</f>
-        <v>0.94807648350964857</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="B5" s="1">
+        <f>'Safety Prob. Systematic Faults'!B29*'Unsafe F. Rate Random Faults'!$C$2</f>
+        <v>1.6588964769984556E-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="23">
-        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$2</f>
-        <v>0.98037402959682518</v>
-      </c>
-      <c r="C6" s="1">
-        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$3</f>
-        <v>0.99065279211809554</v>
-      </c>
-      <c r="D6" s="12">
-        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$4</f>
-        <v>0.99065373893639042</v>
-      </c>
-      <c r="E6" s="12">
-        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$5</f>
-        <v>0.99144594434334732</v>
-      </c>
-      <c r="F6" s="12">
-        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$6</f>
-        <v>0.99144782324788516</v>
-      </c>
-      <c r="G6" s="12">
-        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$7</f>
-        <v>0.99184338648787629</v>
-      </c>
-      <c r="H6" s="12">
-        <f>'Safety Prob. Systematic Faults'!B30*'Safety Prob. Random Faults'!$B$8</f>
-        <v>0.99184707770200642</v>
+      <c r="B6" s="1">
+        <f>'Safety Prob. Systematic Faults'!B30*'Unsafe F. Rate Random Faults'!$C$2</f>
+        <v>1.7354840580267667E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EC1:Final update of the quantitative safety model Finished calculating random and systematic faults for IEC61508:2010 high demand mode (transformation of failure probabilities into failure rates).
</commit_message>
<xml_diff>
--- a/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Quantitative Models/Compiled Safety Results.xlsx
+++ b/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Quantitative Models/Compiled Safety Results.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio\Documents\safetyartist GitHub\EC1-ECG_Analysis\ecg_oversampling\safetyArtist\Quantitative Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Arnaldo\Documents\Documentos Toti\Escola Politécnica - USP\Pós-Graduação\Doutorado\safetyartist\EC1-ECG_Analysis\ecg_oversampling\safetyArtist\Quantitative Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="20730" windowHeight="10050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Safety Prob. Systematic Faults" sheetId="8" r:id="rId1"/>
-    <sheet name="Unsafe F. Rate Random Faults" sheetId="9" r:id="rId2"/>
-    <sheet name="Final Unsafe Failure Rates" sheetId="10" r:id="rId3"/>
+    <sheet name="Safety Sys. Faults F. Rates" sheetId="9" r:id="rId2"/>
+    <sheet name="Global Unsafe Failure Rate" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="56">
   <si>
     <t>ResNet</t>
   </si>
@@ -68,16 +68,127 @@
     <t>Operational Context</t>
   </si>
   <si>
-    <t>Without Preventive Maintenance</t>
-  </si>
-  <si>
-    <t>MTTUF (lower bound)</t>
-  </si>
-  <si>
-    <t>Unsafe Failure Rate (upper bound)</t>
-  </si>
-  <si>
-    <t>Without preventive maintenance</t>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>Number of Short ECGs per Hour</t>
+  </si>
+  <si>
+    <t>Number of Holter ECGs per Day</t>
+  </si>
+  <si>
+    <t>Laboratory Working Hours for Short ECGs</t>
+  </si>
+  <si>
+    <t>Total Heartbeats Analyzed per Day</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 2 Wrong Heartbeats per Short ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 5 Wrong Heartbeats per Holter ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 3 Wrong Heartbeats per Short ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 3 Wrong Heartbeats per Holter ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 2 Wrong Heartbeats per Holter ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 1 Overall Wrong Heartbeat</t>
+  </si>
+  <si>
+    <t>Number of Heartbeats for Unsafe Diagnose</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 1 Wrong Heartbeat per Short ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 1 Wrong Heartbeat per Holter ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 2 Overall Wrong Heartbeats</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 3 Overall Wrong Heartbeats</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 4 Overall Wrong Heartbeats</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 4 Wrong Heartbeats per Short ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 4 Wrong Heartbeats per Holter ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 5 Overall Wrong Heartbeats</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 5 Wrong Heartbeats per Short ECG</t>
+  </si>
+  <si>
+    <t>Average Heartbeat Rate (bpm)</t>
+  </si>
+  <si>
+    <t>Short ECG Duration (min)</t>
+  </si>
+  <si>
+    <t>Holter ECG Duration (min)</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 6 Overall Wrong Heartbeats</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 6 Wrong Heartbeats per Short ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 6 Wrong Heartbeats per Holter ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 7 Overall Wrong Heartbeats</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 7 Wrong Heartbeats per Short ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 7 Wrong Heartbeats per Holter ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 8 Overall Wrong Heartbeats</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 8 Wrong Heartbeats per Short ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 8 Wrong Heartbeats per Holter ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 9 Overall Wrong Heartbeats</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 9 Wrong Heartbeats per Short ECG</t>
+  </si>
+  <si>
+    <t>Overall Failure Rates (failures per hour) - 9 Wrong Heartbeats per Holter ECG</t>
+  </si>
+  <si>
+    <t>Total Heartbeats Analyzed per Hour</t>
+  </si>
+  <si>
+    <t>Total Short ECG Heartbeats Analyzed per Day</t>
+  </si>
+  <si>
+    <t>Total Holter ECG Heartbeats Analyzed per Day</t>
+  </si>
+  <si>
+    <t>Total Holter ECG Heartbeats Analyzed per Hour</t>
+  </si>
+  <si>
+    <t>HW Failure Rate</t>
   </si>
 </sst>
 </file>
@@ -157,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -397,35 +508,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -490,6 +577,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -511,17 +617,786 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="64">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -824,7 +1699,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A25" sqref="A25:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,21 +1710,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="24" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="26"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
@@ -983,21 +1858,21 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="24" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="26"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="14" t="s">
         <v>4</v>
       </c>
@@ -1131,21 +2006,21 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="24" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="26"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="14" t="s">
         <v>4</v>
       </c>
@@ -1279,10 +2154,10 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="28"/>
+      <c r="B25" s="35"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
@@ -1344,43 +2219,1620 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" customWidth="1"/>
+    <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="5" max="5" width="51.28515625" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" customWidth="1"/>
+    <col min="7" max="7" width="39" customWidth="1"/>
+    <col min="8" max="8" width="51.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="23">
+        <v>1</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("C(",$B$12,",",$E1,")")</f>
+        <v>C(289380,1)</v>
+      </c>
+      <c r="H1">
+        <f>$B$12</f>
+        <v>289380</v>
+      </c>
+      <c r="I1" t="str">
+        <f>CONCATENATE("C(",$B$8,",",$E1,")")</f>
+        <v>C(8580,1)</v>
+      </c>
+      <c r="J1">
+        <f>$B$8</f>
+        <v>8580</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE("C(",$B$10,",",$E1,")")</f>
+        <v>C(280800,1)</v>
+      </c>
+      <c r="L1">
+        <f>$B$10</f>
+        <v>280800</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="23">
+        <v>2</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G9" si="0">CONCATENATE("C(",$B$12,",",$E2,")")</f>
+        <v>C(289380,2)</v>
+      </c>
+      <c r="H2">
+        <f>($B$12*($B$12-1))/$E2</f>
+        <v>41870247510</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I9" si="1">CONCATENATE("C(",$B$8,",",$E2,")")</f>
+        <v>C(8580,2)</v>
+      </c>
+      <c r="J2">
+        <f>($B$8*($B$8-1))/$E2</f>
+        <v>36803910</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K9" si="2">CONCATENATE("C(",$B$10,",",$E2,")")</f>
+        <v>C(280800,2)</v>
+      </c>
+      <c r="L2">
+        <f>($B$10*($B$10-1))/$E2</f>
+        <v>39424179600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>24*60</f>
+        <v>1440</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="23">
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>C(289380,3)</v>
+      </c>
+      <c r="H3">
+        <f>($B$12*($B$12-1)*($B$12-2))/FACT($E3)</f>
+        <v>4038776161316260</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="1"/>
+        <v>C(8580,3)</v>
+      </c>
+      <c r="J3">
+        <f>($B$8*($B$8-1)*($B$8-2))/FACT($E3)</f>
+        <v>105234646660</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="2"/>
+        <v>C(280800,3)</v>
+      </c>
+      <c r="L3">
+        <f>($B$10*($B$10-1)*($B$10-2))/FACT($E3)</f>
+        <v>3690076927773600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="23">
+        <v>4</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>C(289380,4)</v>
+      </c>
+      <c r="H4">
+        <f>($B$12*($B$12-1)*($B$12-2)*($B$12-3))/FACT($E4)</f>
+        <v>2.9218223230830382E+20</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v>C(8580,4)</v>
+      </c>
+      <c r="J4">
+        <f>($B$8*($B$8-1)*($B$8-2)*($B$8-3))/FACT($E4)</f>
+        <v>225649391100705</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="2"/>
+        <v>C(280800,4)</v>
+      </c>
+      <c r="L4">
+        <f>($B$10*($B$10-1)*($B$10-2)*($B$10-3))/FACT($E4)</f>
+        <v>2.5904063277201087E+20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="23">
+        <v>5</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>C(289380,5)</v>
+      </c>
+      <c r="H5">
+        <f>($B$12*($B$12-1)*($B$12-2)*($B$12-3)*($B12-4))/FACT($E5)</f>
+        <v>1.6910105131289548E+25</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>C(8580,5)</v>
+      </c>
+      <c r="J5">
+        <f>($B$8*($B$8-1)*($B$8-2)*($B$8-3)*($B12-4))/FACT($E5)</f>
+        <v>1.3059503639831521E+19</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="2"/>
+        <v>C(280800,5)</v>
+      </c>
+      <c r="L5">
+        <f>($B$10*($B$10-1)*($B$10-2)*($B$10-3)*($B12-4))/FACT($E5)</f>
+        <v>1.4992028429806683E+25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1">
-        <v>57179505.361074015</v>
-      </c>
-      <c r="C2" s="1">
-        <f>1/B2</f>
-        <v>1.7488783676690706E-8</v>
+      <c r="B6" s="1">
+        <v>11</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="23">
+        <v>6</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>C(289380,6)</v>
+      </c>
+      <c r="H6">
+        <f>($B$12*($B$12-1)*($B$12-2)*($B$12-3)*($B12-4)*($B$12-5))/FACT($E6)</f>
+        <v>8.1556027872781879E+29</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>C(8580,6)</v>
+      </c>
+      <c r="J6">
+        <f>($B$8*($B$8-1)*($B$8-2)*($B$8-3)*($B12-4)*($B$8-5))/FACT($E6)</f>
+        <v>1.8664207285259216E+22</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="2"/>
+        <v>C(280800,6)</v>
+      </c>
+      <c r="L6">
+        <f>($B$10*($B$10-1)*($B$10-2)*($B$10-3)*($B12-4)*($B$10-5))/FACT($E6)</f>
+        <v>7.0161443715792807E+29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1">
+        <v>65</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="23">
+        <v>7</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>C(289380,7)</v>
+      </c>
+      <c r="H7">
+        <f>($B$12*($B$12-1)*($B$12-2)*($B$12-3)*($B12-4)*($B$12-5)*($B$12-6))/FACT($E7)</f>
+        <v>3.371456287094055E+34</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>C(8580,7)</v>
+      </c>
+      <c r="J7">
+        <f>($B$8*($B$8-1)*($B$8-2)*($B$8-3)*($B12-4)*($B$8-5)*($B$8-6))/FACT($E7)</f>
+        <v>2.2860987609116075E+25</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="2"/>
+        <v>C(280800,7)</v>
+      </c>
+      <c r="L7">
+        <f>($B$10*($B$10-1)*($B$10-2)*($B$10-3)*($B12-4)*($B$10-5)*($B$10-6))/FACT($E7)</f>
+        <v>2.8144160609617609E+34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1">
+        <f>(B4*B6*B2*B7)</f>
+        <v>8580</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="23">
+        <v>8</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>C(289380,8)</v>
+      </c>
+      <c r="H8">
+        <f>($B$12*($B$12-1)*($B$12-2)*($B$12-3)*($B12-4)*($B$12-5)*($B$12-6)*($B$12-7))/FACT($E8)</f>
+        <v>1.219510525206585E+39</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>C(8580,8)</v>
+      </c>
+      <c r="J8">
+        <f>($B$8*($B$8-1)*($B$8-2)*($B$8-3)*($B12-4)*($B$8-5)*($B$8-6)*($B$8-7))/FACT($E8)</f>
+        <v>2.4498405846619012E+28</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="2"/>
+        <v>C(280800,8)</v>
+      </c>
+      <c r="L8">
+        <f>($B$10*($B$10-1)*($B$10-2)*($B$10-3)*($B12-4)*($B$10-5)*($B$10-6)*($B$10-7))/FACT($E8)</f>
+        <v>9.8783541125704456E+38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1">
+        <f>ROUNDUP(B8/24, 0)</f>
+        <v>358</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="23">
+        <v>9</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>C(289380,9)</v>
+      </c>
+      <c r="H9">
+        <f>($B$12*($B$12-1)*($B$12-2)*($B$12-3)*($B12-4)*($B$12-5)*($B$12-6)*($B$12-7)*($B$12-8))/FACT($E9)</f>
+        <v>3.921024441111999E+43</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>C(8580,9)</v>
+      </c>
+      <c r="J9">
+        <f>($B$8*($B$8-1)*($B$8-2)*($B$8-3)*($B12-4)*($B$8-5)*($B$8-6)*($B$8-7)*($B$8-8))/FACT($E9)</f>
+        <v>2.3333370546357577E+31</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="2"/>
+        <v>C(280800,9)</v>
+      </c>
+      <c r="L9">
+        <f>($B$10*($B$10-1)*($B$10-2)*($B$10-3)*($B12-4)*($B$10-5)*($B$10-6)*($B$10-7)*($B$10-8))/FACT($E9)</f>
+        <v>3.0819586755298674E+43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1">
+        <f>(B3*B5*B7)</f>
+        <v>280800</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="24"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1">
+        <f>ROUNDUP(B10/24, 0)</f>
+        <v>11700</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="24"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1">
+        <f>(B4*B6*B2*B7)+(B3*B5*B7)</f>
+        <v>289380</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="24"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1">
+        <f>ROUNDUP(B12/24, 0)</f>
+        <v>12058</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="24"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="G15" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="36"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$26), E$1)</f>
+        <v>690.34823340000037</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$1)</f>
+        <v>20.496323400000012</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$1)</f>
+        <v>669.85191000000043</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$27), E$1)</f>
+        <v>3.0723783999999936</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$1)</f>
+        <v>9.1218399999999811E-2</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$1)</f>
+        <v>2.9811599999999938</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$28), E$1)</f>
+        <v>24.383687599999686</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$1)</f>
+        <v>0.7239475999999907</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$1)</f>
+        <v>23.659739999999697</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$29), E$1)</f>
+        <v>620.39856960000031</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$1)</f>
+        <v>18.419529600000011</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$1)</f>
+        <v>601.9790400000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$30), E$1)</f>
+        <v>92.349810399999583</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$1)</f>
+        <v>2.7418503999999877</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$1)</f>
+        <v>89.607959999999593</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+    </row>
+    <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="36"/>
+      <c r="D22" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="36"/>
+      <c r="G22" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="36"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$26), E$2)</f>
+        <v>39.524024163086871</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$2)</f>
+        <v>1.1734616561938214</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$2)</f>
+        <v>38.350562506893048</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$27), E$2)</f>
+        <v>7.8284201631999674E-4</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$2)</f>
+        <v>2.3242448319999904E-5</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$2)</f>
+        <v>7.5959956799999677E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$28), E$2)</f>
+        <v>4.9308693064718738E-2</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$2)</f>
+        <v>1.4639668367199626E-3</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$2)</f>
+        <v>4.7844726227998777E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$29), E$2)</f>
+        <v>31.920250884203558</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$2)</f>
+        <v>0.94770690135552105</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$2)</f>
+        <v>30.972543982848038</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$30), E$2)</f>
+        <v>0.70728872789151365</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$2)</f>
+        <v>2.0999283843519814E-2</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$2)</f>
+        <v>0.68628944404799386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="D29" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="36"/>
+      <c r="G29" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="36"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$26), E$3)</f>
+        <v>2.2628412885922997</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$3)</f>
+        <v>6.7183378778905567E-2</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$3)</f>
+        <v>2.1956579098133941</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$27), E$3)</f>
+        <v>1.9946814575833475E-7</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$3)</f>
+        <v>5.9221758319359626E-9</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$3)</f>
+        <v>1.9354596992639877E-7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$28), E$3)</f>
+        <v>9.9712039115472942E-5</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$3)</f>
+        <v>2.9604337372150701E-6</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$3)</f>
+        <v>9.6751605378257881E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$29), E$3)</f>
+        <v>1.6423352122933352</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$3)</f>
+        <v>4.8760657323023218E-2</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$3)</f>
+        <v>1.593574554970312</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$30), E$3)</f>
+        <v>5.4169829091755004E-3</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$3)</f>
+        <v>1.608293151007488E-4</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$3)</f>
+        <v>5.2561535940747516E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="36"/>
+      <c r="D36" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="36"/>
+      <c r="G36" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="36"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$26), E$4)</f>
+        <v>0.12955286830687301</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$4)</f>
+        <v>3.8464029568635377E-3</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$4)</f>
+        <v>0.12570646535000948</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$27), E$4)</f>
+        <v>5.0824483539223585E-11</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$4)</f>
+        <v>1.5089704019772801E-12</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$4)</f>
+        <v>4.9315513137246303E-11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$28), E$4)</f>
+        <v>2.016376854993068E-7</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$4)</f>
+        <v>5.986589103396238E-9</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$4)</f>
+        <v>1.9565109639591057E-7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$29), E$4)</f>
+        <v>8.450011747474688E-2</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$4)</f>
+        <v>2.5087943320583335E-3</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H40" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$4)</f>
+        <v>8.1991323142688546E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$30), E$4)</f>
+        <v>4.1487588704793143E-5</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$4)</f>
+        <v>1.2317595584936096E-6</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$4)</f>
+        <v>4.0255829146299532E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="36"/>
+      <c r="D43" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="36"/>
+      <c r="G43" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" s="36"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$26), E$5)</f>
+        <v>7.4171996821655898E-3</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$5)</f>
+        <v>2.2021541600723846E-4</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$5)</f>
+        <v>7.1969842661583515E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$27), E$5)</f>
+        <v>1.2950078405794142E-14</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$5)</f>
+        <v>3.8448565842381016E-16</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$5)</f>
+        <v>1.2565592747370332E-14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$28), E$5)</f>
+        <v>4.0775172761669296E-10</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$5)</f>
+        <v>1.2106080484887715E-11</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H46" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$5)</f>
+        <v>3.9564564713180523E-10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$29), E$5)</f>
+        <v>4.3476324442166996E-3</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$5)</f>
+        <v>1.2908047893759982E-4</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H47" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$5)</f>
+        <v>4.2185519652790998E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$30), E$5)</f>
+        <v>3.1774514437226829E-7</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$5)</f>
+        <v>9.4338001065908141E-9</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$5)</f>
+        <v>3.0831134426567749E-7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="36"/>
+      <c r="D50" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="36"/>
+      <c r="G50" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H50" s="36"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$26), E$6)</f>
+        <v>4.2465174136324928E-4</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$6)</f>
+        <v>1.2607839061871227E-5</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$6)</f>
+        <v>4.120439023013781E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$27), E$6)</f>
+        <v>3.29967997779634E-18</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$6)</f>
+        <v>9.7966945766386617E-20</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$6)</f>
+        <v>3.2017130320299536E-18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$28), E$6)</f>
+        <v>8.2455554358646595E-13</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$6)</f>
+        <v>2.4480915956539626E-14</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H53" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$6)</f>
+        <v>8.0007462762992633E-13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$29), E$6)</f>
+        <v>2.2369090641388237E-4</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$6)</f>
+        <v>6.641345537914238E-6</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H54" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$6)</f>
+        <v>2.1704956087596812E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$30), E$6)</f>
+        <v>2.4335465117183173E-9</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$6)</f>
+        <v>7.2251588256357407E-11</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$6)</f>
+        <v>2.36129492346196E-9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="36"/>
+      <c r="D57" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" s="36"/>
+      <c r="G57" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="H57" s="36"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$26), E$7)</f>
+        <v>2.4312288892051171E-5</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$7)</f>
+        <v>7.2182778432197047E-7</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$7)</f>
+        <v>2.3590461107729202E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$27), E$7)</f>
+        <v>8.4075845834250586E-22</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$7)</f>
+        <v>2.4961977781275259E-23</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$7)</f>
+        <v>8.1579648056123059E-22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$28), E$7)</f>
+        <v>1.6674162202405301E-15</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$7)</f>
+        <v>4.9505308247313798E-17</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H60" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$7)</f>
+        <v>1.6179109119932164E-15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$29), E$7)</f>
+        <v>1.1509165564081951E-5</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$7)</f>
+        <v>3.4170519754033328E-7</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H61" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$7)</f>
+        <v>1.1167460366541619E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$30), E$7)</f>
+        <v>1.8638046023948164E-11</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$7)</f>
+        <v>5.5336046413778767E-13</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$7)</f>
+        <v>1.8084685559810377E-11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="36"/>
+      <c r="D64" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E64" s="36"/>
+      <c r="G64" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H64" s="36"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$26), E$8)</f>
+        <v>1.3919344573343821E-6</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$8)</f>
+        <v>4.1326300856336776E-8</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$8)</f>
+        <v>1.3506081564780453E-6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$27), E$8)</f>
+        <v>2.1422525518566998E-25</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$8)</f>
+        <v>6.3603119386689216E-27</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H66" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$8)</f>
+        <v>2.0786494324700105E-25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$28), E$8)</f>
+        <v>3.3718490805703563E-18</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$8)</f>
+        <v>1.0010963433771667E-19</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H67" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$8)</f>
+        <v>3.2717394462326398E-18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$29), E$8)</f>
+        <v>5.921603792706936E-7</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$8)</f>
+        <v>1.7581142459687205E-8</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H68" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$8)</f>
+        <v>5.7457923681100634E-7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$30), E$8)</f>
+        <v>1.4274506688821357E-13</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$8)</f>
+        <v>4.2380771227384693E-15</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H69" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$8)</f>
+        <v>1.3850698976547512E-13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="36"/>
+      <c r="D71" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71" s="36"/>
+      <c r="G71" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="H71" s="36"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$26), E$9)</f>
+        <v>7.9691449131645301E-8</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$9)</f>
+        <v>2.3660257745172514E-9</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H72" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$26), $E$9)</f>
+        <v>7.7325423357128041E-8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$27), E$9)</f>
+        <v>5.4584595021308597E-29</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$9)</f>
+        <v>1.620607481972838E-30</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H73" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$27), $E$9)</f>
+        <v>5.2963987539335762E-29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$28), E$9)</f>
+        <v>6.8185532107292875E-21</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$9)</f>
+        <v>2.0244170255772805E-22</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H74" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$28), $E$9)</f>
+        <v>6.6161115081715594E-21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$29), E$9)</f>
+        <v>3.046736210593233E-8</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$9)</f>
+        <v>9.045708769218588E-10</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H75" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$29), $E$9)</f>
+        <v>2.9562791229010469E-8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="1">
+        <f>(B$13)*POWER((1-'Safety Prob. Systematic Faults'!$B$30), E$9)</f>
+        <v>1.0932559182834453E-15</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="1">
+        <f>$B$9*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$9)</f>
+        <v>3.2458585067629246E-17</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="1">
+        <f>$B$11*POWER((1-'Safety Prob. Systematic Faults'!$B$30), $E$9)</f>
+        <v>1.060797333215816E-15</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="D1:D9"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="G64:H64"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B16:B20 B23:B27 E16:E20 E23:E27 H23:H27 H16:H20 E30:E34 H30:H34 B30:B34 B37:B41 B44:B48 B51:B55 E37:E41 E44:E48 E51:E55 H37:H41 H44:H48 H51:H55 B58:B62 B65:B69 B72:B76 E58:E62 E65:E69 E72:E76 H58:H62 H65:H69 H72:H76">
+    <cfRule type="cellIs" dxfId="61" priority="1" operator="greaterThanOrEqual">
+      <formula>0.0000001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="2" operator="lessThan">
+      <formula>0.0000001</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1388,72 +3840,1253 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="54.28515625" customWidth="1"/>
+    <col min="6" max="6" width="2" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" customWidth="1"/>
+    <col min="8" max="8" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <f>'Safety Prob. Systematic Faults'!B26*'Unsafe F. Rate Random Faults'!$C$2</f>
-        <v>1.6487510586997705E-8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <f>'Safety Prob. Systematic Faults'!B27*'Unsafe F. Rate Random Faults'!$C$2</f>
-        <v>1.7484327534609885E-8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1.7488800000000001E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="36"/>
+      <c r="G3" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="36"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1">
-        <f>'Safety Prob. Systematic Faults'!B28*'Unsafe F. Rate Random Faults'!$C$2</f>
-        <v>1.7453417858339704E-8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B16</f>
+        <v>690.34823341748915</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E16</f>
+        <v>20.496323417488814</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H16</f>
+        <v>669.85191001748922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1">
-        <f>'Safety Prob. Systematic Faults'!B29*'Unsafe F. Rate Random Faults'!$C$2</f>
-        <v>1.6588964769984556E-8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B17</f>
+        <v>3.0723784174887938</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E17</f>
+        <v>9.1218417488799816E-2</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H17</f>
+        <v>2.981160017488794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1">
-        <f>'Safety Prob. Systematic Faults'!B30*'Unsafe F. Rate Random Faults'!$C$2</f>
-        <v>1.7354840580267667E-8</v>
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B18</f>
+        <v>24.383687617488487</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E18</f>
+        <v>0.72394761748879066</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H18</f>
+        <v>23.659740017488499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B19</f>
+        <v>620.3985696174891</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E19</f>
+        <v>18.419529617488813</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H19</f>
+        <v>601.97904001748918</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B20</f>
+        <v>92.349810417488385</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E20</f>
+        <v>2.7418504174887879</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H20</f>
+        <v>89.607960017488395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="D10" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="G10" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="36"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B23</f>
+        <v>39.524024180575672</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E23</f>
+        <v>1.1734616736826213</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H23</f>
+        <v>38.35056252438185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B24</f>
+        <v>7.8285950511999673E-4</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E24</f>
+        <v>2.3259937119999905E-5</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H24</f>
+        <v>7.5961705679999676E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B25</f>
+        <v>4.9308710553518736E-2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E25</f>
+        <v>1.4639843255199625E-3</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H25</f>
+        <v>4.7844743716798775E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B26</f>
+        <v>31.920250901692359</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E26</f>
+        <v>0.94770691884432101</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H26</f>
+        <v>30.972544000336839</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B27</f>
+        <v>0.70728874538031361</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E27</f>
+        <v>2.0999301332319812E-2</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H27</f>
+        <v>0.68628946153679382</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="D17" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="36"/>
+      <c r="G17" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="36"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B30</f>
+        <v>2.2628413060810999</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E30</f>
+        <v>6.7183396267705572E-2</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H30</f>
+        <v>2.1956579273021943</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B31</f>
+        <v>2.1695694575833474E-7</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E31</f>
+        <v>2.3410975831935964E-8</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H31</f>
+        <v>2.1103476992639876E-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B32</f>
+        <v>9.972952791547294E-5</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E32</f>
+        <v>2.9779225372150699E-6</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H32</f>
+        <v>9.6769094178257879E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B33</f>
+        <v>1.6423352297821352</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E33</f>
+        <v>4.8760674811823217E-2</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H33</f>
+        <v>1.5935745724591119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B34</f>
+        <v>5.4170003979755006E-3</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E34</f>
+        <v>1.6084680390074881E-4</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H34</f>
+        <v>5.2561710828747518E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="36"/>
+      <c r="D24" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="36"/>
+      <c r="G24" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="36"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B37</f>
+        <v>0.12955288579567301</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E37</f>
+        <v>3.8464204456635379E-3</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H37</f>
+        <v>0.12570648283880947</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B38</f>
+        <v>1.7539624483539226E-8</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E38</f>
+        <v>1.7490308970401978E-8</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H38</f>
+        <v>1.7538115513137246E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B39</f>
+        <v>2.191264854993068E-7</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E39</f>
+        <v>2.3475389103396238E-8</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H39</f>
+        <v>2.1313989639591057E-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B40</f>
+        <v>8.4500134963546886E-2</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E40</f>
+        <v>2.5088118208583337E-3</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H40</f>
+        <v>8.1991340631488552E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B41</f>
+        <v>4.1505077504793141E-5</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E41</f>
+        <v>1.2492483584936096E-6</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H41</f>
+        <v>4.0273317946299529E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="36"/>
+      <c r="D31" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="36"/>
+      <c r="G31" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="36"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B44</f>
+        <v>7.41721717096559E-3</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E44</f>
+        <v>2.2023290480723847E-4</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H44</f>
+        <v>7.1970017549583517E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B45</f>
+        <v>1.7488812950078408E-8</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E45</f>
+        <v>1.748880038448566E-8</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H45</f>
+        <v>1.7488812565592749E-8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B46</f>
+        <v>1.7896551727616694E-8</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E46</f>
+        <v>1.7500906080484888E-8</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H46</f>
+        <v>1.7884445647131805E-8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B47</f>
+        <v>4.3476499330166998E-3</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E47</f>
+        <v>1.2909796773759983E-4</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H47</f>
+        <v>4.2185694540791E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B48</f>
+        <v>3.3523394437226831E-7</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E48</f>
+        <v>2.6922600106590815E-8</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H48</f>
+        <v>3.2580014426567751E-7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="36"/>
+      <c r="D38" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="36"/>
+      <c r="G38" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H38" s="36"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B51</f>
+        <v>4.2466923016324927E-4</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E51</f>
+        <v>1.2625327861871226E-5</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H51</f>
+        <v>4.1206139110137809E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B52</f>
+        <v>1.7488800003299681E-8</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E52</f>
+        <v>1.7488800000097969E-8</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H52</f>
+        <v>1.7488800003201713E-8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B53</f>
+        <v>1.7489624555543587E-8</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E53</f>
+        <v>1.7488824480915958E-8</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H53</f>
+        <v>1.7489600074627631E-8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B54</f>
+        <v>2.2370839521388238E-4</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E54</f>
+        <v>6.6588343379142383E-6</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H54</f>
+        <v>2.1706704967596813E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B55</f>
+        <v>1.9922346511718318E-8</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E55</f>
+        <v>1.7561051588256359E-8</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H55</f>
+        <v>1.985009492346196E-8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="36"/>
+      <c r="D45" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="36"/>
+      <c r="G45" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="H45" s="36"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B58</f>
+        <v>2.4329777692051172E-5</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E58</f>
+        <v>7.3931658432197043E-7</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H58</f>
+        <v>2.3607949907729203E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B59</f>
+        <v>1.7488800000000841E-8</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E59</f>
+        <v>1.7488800000000028E-8</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H59</f>
+        <v>1.7488800000000818E-8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B60</f>
+        <v>1.7488801667416221E-8</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E60</f>
+        <v>1.7488800049505308E-8</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H48" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H60</f>
+        <v>1.7488801617910914E-8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B61</f>
+        <v>1.1526654364081951E-5</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E61</f>
+        <v>3.591939975403333E-7</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H49" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H61</f>
+        <v>1.1184949166541618E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B62</f>
+        <v>1.7507438046023949E-8</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E62</f>
+        <v>1.748935336046414E-8</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H62</f>
+        <v>1.7506884685559813E-8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="36"/>
+      <c r="D52" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="36"/>
+      <c r="G52" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H52" s="36"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B65</f>
+        <v>1.4094232573343821E-6</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E65</f>
+        <v>5.8815100856336777E-8</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H65</f>
+        <v>1.3680969564780453E-6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B66</f>
+        <v>1.7488800000000001E-8</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E66</f>
+        <v>1.7488800000000001E-8</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H54" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H66</f>
+        <v>1.7488800000000001E-8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B67</f>
+        <v>1.7488800003371851E-8</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E67</f>
+        <v>1.748880000010011E-8</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H55" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H67</f>
+        <v>1.7488800003271742E-8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B68</f>
+        <v>6.0964917927069357E-7</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E68</f>
+        <v>3.5069942459687206E-8</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H56" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H68</f>
+        <v>5.9206803681100631E-7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B69</f>
+        <v>1.7488942745066889E-8</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E69</f>
+        <v>1.7488804238077124E-8</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H69</f>
+        <v>1.7488938506989766E-8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="36"/>
+      <c r="D59" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" s="36"/>
+      <c r="G59" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="H59" s="36"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B72</f>
+        <v>9.7180249131645309E-8</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E72</f>
+        <v>1.9854825774517254E-8</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H72</f>
+        <v>9.4814223357128049E-8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B73</f>
+        <v>1.7488800000000001E-8</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E73</f>
+        <v>1.7488800000000001E-8</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H73</f>
+        <v>1.7488800000000001E-8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B74</f>
+        <v>1.748880000000682E-8</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E74</f>
+        <v>1.7488800000000203E-8</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H62" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H74</f>
+        <v>1.7488800000006619E-8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B75</f>
+        <v>4.7956162105932331E-8</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E75</f>
+        <v>1.8393370876921858E-8</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H63" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H75</f>
+        <v>4.7051591229010474E-8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!B76</f>
+        <v>1.748880109325592E-8</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!E76</f>
+        <v>1.7488800032458585E-8</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="1">
+        <f>$B$1+'Safety Sys. Faults F. Rates'!H76</f>
+        <v>1.7488801060797333E-8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G10:H10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B4:B8 E4:E8 H4:H8 B11:B15 E11:E15 H11:H15 B18:B22 E18:E22 H18:H22 B25:B29 E25:E29 H25:H29 B32:B36 E32:E36 H32:H36 B39:B43 E39:E43 H39:H43 B46:B50 E46:E50 H46:H50 B53:B57 E53:E57 H53:H57 B60:B64 E60:E64 H60:H64">
+    <cfRule type="cellIs" dxfId="59" priority="3" operator="greaterThanOrEqual">
+      <formula>0.0000001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="4" operator="lessThan">
+      <formula>0.0000001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="greaterThanOrEqual">
+      <formula>0.0000001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="2" operator="lessThan">
+      <formula>0.0000001</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>